<commit_message>
Adding phenology data into observations
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/Dookie2024.xlsx
+++ b/Tests/Validation/Wheat/data/Dookie2024.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="22">
   <si>
     <t>Wheat.Height</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Wheat.Phenology.HaunStage</t>
+  </si>
+  <si>
+    <t>Wheat.Phenology.Stage</t>
   </si>
   <si>
     <t>SimulationName</t>
@@ -440,18 +443,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E357"/>
+  <dimension ref="A1:F405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -462,10 +465,13 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>45443</v>
@@ -474,9 +480,9 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>45460</v>
@@ -485,9 +491,9 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>45474</v>
@@ -496,9 +502,9 @@
         <v>0.2425</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>45487</v>
@@ -507,9 +513,9 @@
         <v>0.3425</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>45502</v>
@@ -518,9 +524,9 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>45513</v>
@@ -529,9 +535,9 @@
         <v>0.5475</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>45526</v>
@@ -540,9 +546,9 @@
         <v>0.6775</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2">
         <v>45548</v>
@@ -551,9 +557,9 @@
         <v>0.835</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>45559</v>
@@ -562,9 +568,9 @@
         <v>0.7925</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2">
         <v>45571</v>
@@ -573,9 +579,9 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
         <v>45582</v>
@@ -584,9 +590,9 @@
         <v>0.5775</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2">
         <v>45594</v>
@@ -595,9 +601,9 @@
         <v>0.385</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2">
         <v>45609</v>
@@ -606,9 +612,9 @@
         <v>0.1125</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2">
         <v>45443</v>
@@ -617,9 +623,9 @@
         <v>0.285</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2">
         <v>45460</v>
@@ -630,7 +636,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" s="2">
         <v>45474</v>
@@ -641,7 +647,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" s="2">
         <v>45487</v>
@@ -652,7 +658,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19" s="2">
         <v>45502</v>
@@ -663,7 +669,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20" s="2">
         <v>45513</v>
@@ -674,7 +680,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" s="2">
         <v>45526</v>
@@ -685,7 +691,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B22" s="2">
         <v>45548</v>
@@ -696,7 +702,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B23" s="2">
         <v>45559</v>
@@ -707,7 +713,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B24" s="2">
         <v>45571</v>
@@ -718,7 +724,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B25" s="2">
         <v>45582</v>
@@ -729,7 +735,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B26" s="2">
         <v>45594</v>
@@ -740,7 +746,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B27" s="2">
         <v>45609</v>
@@ -751,7 +757,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B28" s="2">
         <v>45443</v>
@@ -762,7 +768,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B29" s="2">
         <v>45460</v>
@@ -773,7 +779,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B30" s="2">
         <v>45474</v>
@@ -784,7 +790,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B31" s="2">
         <v>45487</v>
@@ -795,7 +801,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B32" s="2">
         <v>45502</v>
@@ -806,7 +812,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B33" s="2">
         <v>45513</v>
@@ -817,7 +823,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B34" s="2">
         <v>45526</v>
@@ -828,7 +834,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B35" s="2">
         <v>45548</v>
@@ -839,7 +845,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B36" s="2">
         <v>45559</v>
@@ -850,7 +856,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B37" s="2">
         <v>45571</v>
@@ -861,7 +867,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B38" s="2">
         <v>45582</v>
@@ -872,7 +878,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B39" s="2">
         <v>45594</v>
@@ -883,7 +889,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B40" s="2">
         <v>45609</v>
@@ -894,7 +900,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B41" s="2">
         <v>45443</v>
@@ -905,7 +911,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B42" s="2">
         <v>45460</v>
@@ -916,7 +922,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B43" s="2">
         <v>45474</v>
@@ -927,7 +933,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B44" s="2">
         <v>45487</v>
@@ -938,7 +944,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B45" s="2">
         <v>45502</v>
@@ -949,7 +955,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B46" s="2">
         <v>45513</v>
@@ -960,7 +966,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B47" s="2">
         <v>45526</v>
@@ -971,7 +977,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B48" s="2">
         <v>45548</v>
@@ -982,7 +988,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B49" s="2">
         <v>45559</v>
@@ -993,7 +999,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B50" s="2">
         <v>45571</v>
@@ -1004,7 +1010,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B51" s="2">
         <v>45582</v>
@@ -1015,7 +1021,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B52" s="2">
         <v>45594</v>
@@ -1026,7 +1032,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B53" s="2">
         <v>45609</v>
@@ -1037,7 +1043,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B54" s="2">
         <v>45443</v>
@@ -1048,7 +1054,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B55" s="2">
         <v>45460</v>
@@ -1059,7 +1065,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B56" s="2">
         <v>45474</v>
@@ -1070,7 +1076,7 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B57" s="2">
         <v>45487</v>
@@ -1081,7 +1087,7 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B58" s="2">
         <v>45502</v>
@@ -1092,7 +1098,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B59" s="2">
         <v>45513</v>
@@ -1103,7 +1109,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B60" s="2">
         <v>45526</v>
@@ -1114,7 +1120,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B61" s="2">
         <v>45548</v>
@@ -1125,7 +1131,7 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B62" s="2">
         <v>45559</v>
@@ -1136,7 +1142,7 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B63" s="2">
         <v>45571</v>
@@ -1147,7 +1153,7 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B64" s="2">
         <v>45582</v>
@@ -1158,7 +1164,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B65" s="2">
         <v>45594</v>
@@ -1169,7 +1175,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B66" s="2">
         <v>45609</v>
@@ -1180,7 +1186,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B67" s="2">
         <v>45443</v>
@@ -1191,7 +1197,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B68" s="2">
         <v>45460</v>
@@ -1202,7 +1208,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B69" s="2">
         <v>45474</v>
@@ -1213,7 +1219,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B70" s="2">
         <v>45487</v>
@@ -1224,7 +1230,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B71" s="2">
         <v>45502</v>
@@ -1235,7 +1241,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B72" s="2">
         <v>45513</v>
@@ -1246,7 +1252,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B73" s="2">
         <v>45526</v>
@@ -1257,7 +1263,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B74" s="2">
         <v>45548</v>
@@ -1268,7 +1274,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B75" s="2">
         <v>45559</v>
@@ -1279,7 +1285,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B76" s="2">
         <v>45571</v>
@@ -1290,7 +1296,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B77" s="2">
         <v>45582</v>
@@ -1301,7 +1307,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B78" s="2">
         <v>45594</v>
@@ -1312,7 +1318,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B79" s="2">
         <v>45609</v>
@@ -1323,7 +1329,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B80" s="2">
         <v>45443</v>
@@ -1334,7 +1340,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B81" s="2">
         <v>45460</v>
@@ -1345,7 +1351,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B82" s="2">
         <v>45474</v>
@@ -1356,7 +1362,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B83" s="2">
         <v>45487</v>
@@ -1367,7 +1373,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B84" s="2">
         <v>45502</v>
@@ -1378,7 +1384,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B85" s="2">
         <v>45513</v>
@@ -1389,7 +1395,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B86" s="2">
         <v>45526</v>
@@ -1400,7 +1406,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B87" s="2">
         <v>45548</v>
@@ -1411,7 +1417,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B88" s="2">
         <v>45559</v>
@@ -1422,7 +1428,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B89" s="2">
         <v>45571</v>
@@ -1433,7 +1439,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B90" s="2">
         <v>45582</v>
@@ -1444,7 +1450,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B91" s="2">
         <v>45594</v>
@@ -1455,7 +1461,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B92" s="2">
         <v>45609</v>
@@ -1466,7 +1472,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B93" s="2">
         <v>45443</v>
@@ -1477,7 +1483,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B94" s="2">
         <v>45460</v>
@@ -1488,7 +1494,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B95" s="2">
         <v>45474</v>
@@ -1499,7 +1505,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B96" s="2">
         <v>45487</v>
@@ -1510,7 +1516,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B97" s="2">
         <v>45502</v>
@@ -1521,7 +1527,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B98" s="2">
         <v>45513</v>
@@ -1532,7 +1538,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B99" s="2">
         <v>45526</v>
@@ -1543,7 +1549,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B100" s="2">
         <v>45548</v>
@@ -1554,7 +1560,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B101" s="2">
         <v>45559</v>
@@ -1565,7 +1571,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B102" s="2">
         <v>45571</v>
@@ -1576,7 +1582,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B103" s="2">
         <v>45582</v>
@@ -1587,7 +1593,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B104" s="2">
         <v>45594</v>
@@ -1598,7 +1604,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B105" s="2">
         <v>45609</v>
@@ -1609,7 +1615,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B106" s="2">
         <v>45443</v>
@@ -1620,7 +1626,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B107" s="2">
         <v>45460</v>
@@ -1631,7 +1637,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B108" s="2">
         <v>45474</v>
@@ -1642,7 +1648,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B109" s="2">
         <v>45487</v>
@@ -1653,7 +1659,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B110" s="2">
         <v>45502</v>
@@ -1664,7 +1670,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B111" s="2">
         <v>45513</v>
@@ -1675,7 +1681,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B112" s="2">
         <v>45526</v>
@@ -1686,7 +1692,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B113" s="2">
         <v>45548</v>
@@ -1697,7 +1703,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B114" s="2">
         <v>45559</v>
@@ -1708,7 +1714,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B115" s="2">
         <v>45571</v>
@@ -1719,7 +1725,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B116" s="2">
         <v>45582</v>
@@ -1730,7 +1736,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B117" s="2">
         <v>45594</v>
@@ -1741,7 +1747,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B118" s="2">
         <v>45609</v>
@@ -1752,7 +1758,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B119" s="2">
         <v>45443</v>
@@ -1763,7 +1769,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B120" s="2">
         <v>45460</v>
@@ -1774,7 +1780,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B121" s="2">
         <v>45474</v>
@@ -1785,7 +1791,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B122" s="2">
         <v>45487</v>
@@ -1796,7 +1802,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B123" s="2">
         <v>45502</v>
@@ -1807,7 +1813,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B124" s="2">
         <v>45513</v>
@@ -1818,7 +1824,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B125" s="2">
         <v>45526</v>
@@ -1829,7 +1835,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B126" s="2">
         <v>45548</v>
@@ -1840,7 +1846,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B127" s="2">
         <v>45559</v>
@@ -1851,7 +1857,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B128" s="2">
         <v>45571</v>
@@ -1862,7 +1868,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B129" s="2">
         <v>45582</v>
@@ -1873,7 +1879,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B130" s="2">
         <v>45594</v>
@@ -1884,7 +1890,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B131" s="2">
         <v>45609</v>
@@ -1895,7 +1901,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B132" s="2">
         <v>45443</v>
@@ -1906,7 +1912,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B133" s="2">
         <v>45460</v>
@@ -1917,7 +1923,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B134" s="2">
         <v>45474</v>
@@ -1928,7 +1934,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B135" s="2">
         <v>45487</v>
@@ -1939,7 +1945,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B136" s="2">
         <v>45502</v>
@@ -1950,7 +1956,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B137" s="2">
         <v>45513</v>
@@ -1961,7 +1967,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B138" s="2">
         <v>45526</v>
@@ -1972,7 +1978,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B139" s="2">
         <v>45548</v>
@@ -1983,7 +1989,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B140" s="2">
         <v>45559</v>
@@ -1994,7 +2000,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B141" s="2">
         <v>45571</v>
@@ -2005,7 +2011,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B142" s="2">
         <v>45582</v>
@@ -2016,7 +2022,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B143" s="2">
         <v>45594</v>
@@ -2027,7 +2033,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B144" s="2">
         <v>45609</v>
@@ -2038,7 +2044,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B145" s="2">
         <v>45443</v>
@@ -2049,7 +2055,7 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B146" s="2">
         <v>45460</v>
@@ -2060,7 +2066,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B147" s="2">
         <v>45474</v>
@@ -2071,7 +2077,7 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B148" s="2">
         <v>45487</v>
@@ -2082,7 +2088,7 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B149" s="2">
         <v>45502</v>
@@ -2093,7 +2099,7 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B150" s="2">
         <v>45513</v>
@@ -2104,7 +2110,7 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B151" s="2">
         <v>45526</v>
@@ -2115,7 +2121,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B152" s="2">
         <v>45548</v>
@@ -2126,7 +2132,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B153" s="2">
         <v>45559</v>
@@ -2137,7 +2143,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B154" s="2">
         <v>45571</v>
@@ -2148,7 +2154,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B155" s="2">
         <v>45582</v>
@@ -2159,7 +2165,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B156" s="2">
         <v>45594</v>
@@ -2170,7 +2176,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B157" s="2">
         <v>45609</v>
@@ -2181,7 +2187,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B158" s="2">
         <v>45443</v>
@@ -2192,7 +2198,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B159" s="2">
         <v>45460</v>
@@ -2203,7 +2209,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B160" s="2">
         <v>45474</v>
@@ -2214,7 +2220,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B161" s="2">
         <v>45487</v>
@@ -2225,7 +2231,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B162" s="2">
         <v>45502</v>
@@ -2236,7 +2242,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B163" s="2">
         <v>45513</v>
@@ -2247,7 +2253,7 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B164" s="2">
         <v>45526</v>
@@ -2258,7 +2264,7 @@
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B165" s="2">
         <v>45548</v>
@@ -2269,7 +2275,7 @@
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B166" s="2">
         <v>45559</v>
@@ -2280,7 +2286,7 @@
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B167" s="2">
         <v>45571</v>
@@ -2291,7 +2297,7 @@
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B168" s="2">
         <v>45582</v>
@@ -2302,7 +2308,7 @@
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B169" s="2">
         <v>45594</v>
@@ -2313,7 +2319,7 @@
     </row>
     <row r="170" spans="1:4">
       <c r="A170" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B170" s="2">
         <v>45609</v>
@@ -2324,7 +2330,7 @@
     </row>
     <row r="171" spans="1:4">
       <c r="A171" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B171" s="2">
         <v>45443</v>
@@ -2335,7 +2341,7 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B172" s="2">
         <v>45460</v>
@@ -2346,7 +2352,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B173" s="2">
         <v>45474</v>
@@ -2357,7 +2363,7 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B174" s="2">
         <v>45487</v>
@@ -2368,7 +2374,7 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B175" s="2">
         <v>45502</v>
@@ -2379,7 +2385,7 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B176" s="2">
         <v>45513</v>
@@ -2390,7 +2396,7 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B177" s="2">
         <v>45526</v>
@@ -2401,7 +2407,7 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B178" s="2">
         <v>45548</v>
@@ -2412,7 +2418,7 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B179" s="2">
         <v>45559</v>
@@ -2423,7 +2429,7 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B180" s="2">
         <v>45571</v>
@@ -2434,7 +2440,7 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B181" s="2">
         <v>45582</v>
@@ -2445,7 +2451,7 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B182" s="2">
         <v>45594</v>
@@ -2456,7 +2462,7 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B183" s="2">
         <v>45609</v>
@@ -2467,7 +2473,7 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B184" s="2">
         <v>45443</v>
@@ -2478,7 +2484,7 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B185" s="2">
         <v>45460</v>
@@ -2489,7 +2495,7 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B186" s="2">
         <v>45474</v>
@@ -2500,7 +2506,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B187" s="2">
         <v>45487</v>
@@ -2511,7 +2517,7 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B188" s="2">
         <v>45502</v>
@@ -2522,7 +2528,7 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B189" s="2">
         <v>45513</v>
@@ -2533,7 +2539,7 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B190" s="2">
         <v>45526</v>
@@ -2544,7 +2550,7 @@
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B191" s="2">
         <v>45548</v>
@@ -2555,7 +2561,7 @@
     </row>
     <row r="192" spans="1:4">
       <c r="A192" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B192" s="2">
         <v>45559</v>
@@ -2566,7 +2572,7 @@
     </row>
     <row r="193" spans="1:4">
       <c r="A193" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B193" s="2">
         <v>45571</v>
@@ -2577,7 +2583,7 @@
     </row>
     <row r="194" spans="1:4">
       <c r="A194" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B194" s="2">
         <v>45582</v>
@@ -2588,7 +2594,7 @@
     </row>
     <row r="195" spans="1:4">
       <c r="A195" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B195" s="2">
         <v>45594</v>
@@ -2599,7 +2605,7 @@
     </row>
     <row r="196" spans="1:4">
       <c r="A196" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B196" s="2">
         <v>45609</v>
@@ -2610,7 +2616,7 @@
     </row>
     <row r="197" spans="1:4">
       <c r="A197" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B197" s="2">
         <v>45443</v>
@@ -2621,7 +2627,7 @@
     </row>
     <row r="198" spans="1:4">
       <c r="A198" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B198" s="2">
         <v>45460</v>
@@ -2632,7 +2638,7 @@
     </row>
     <row r="199" spans="1:4">
       <c r="A199" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B199" s="2">
         <v>45474</v>
@@ -2643,7 +2649,7 @@
     </row>
     <row r="200" spans="1:4">
       <c r="A200" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B200" s="2">
         <v>45487</v>
@@ -2654,7 +2660,7 @@
     </row>
     <row r="201" spans="1:4">
       <c r="A201" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B201" s="2">
         <v>45502</v>
@@ -2665,7 +2671,7 @@
     </row>
     <row r="202" spans="1:4">
       <c r="A202" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B202" s="2">
         <v>45513</v>
@@ -2676,7 +2682,7 @@
     </row>
     <row r="203" spans="1:4">
       <c r="A203" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B203" s="2">
         <v>45526</v>
@@ -2687,7 +2693,7 @@
     </row>
     <row r="204" spans="1:4">
       <c r="A204" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B204" s="2">
         <v>45548</v>
@@ -2698,7 +2704,7 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B205" s="2">
         <v>45559</v>
@@ -2709,7 +2715,7 @@
     </row>
     <row r="206" spans="1:4">
       <c r="A206" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B206" s="2">
         <v>45571</v>
@@ -2720,7 +2726,7 @@
     </row>
     <row r="207" spans="1:4">
       <c r="A207" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B207" s="2">
         <v>45582</v>
@@ -2731,7 +2737,7 @@
     </row>
     <row r="208" spans="1:4">
       <c r="A208" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B208" s="2">
         <v>45594</v>
@@ -2742,7 +2748,7 @@
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B209" s="2">
         <v>45609</v>
@@ -2753,7 +2759,7 @@
     </row>
     <row r="210" spans="1:5">
       <c r="A210" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B210" s="2">
         <v>45467</v>
@@ -2764,7 +2770,7 @@
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B211" s="2">
         <v>45477</v>
@@ -2775,7 +2781,7 @@
     </row>
     <row r="212" spans="1:5">
       <c r="A212" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B212" s="2">
         <v>45488</v>
@@ -2786,7 +2792,7 @@
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B213" s="2">
         <v>45499</v>
@@ -2797,7 +2803,7 @@
     </row>
     <row r="214" spans="1:5">
       <c r="A214" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B214" s="2">
         <v>45513</v>
@@ -2808,7 +2814,7 @@
     </row>
     <row r="215" spans="1:5">
       <c r="A215" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B215" s="2">
         <v>45523</v>
@@ -2819,7 +2825,7 @@
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B216" s="2">
         <v>45535</v>
@@ -2830,7 +2836,7 @@
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B217" s="2">
         <v>45549</v>
@@ -2841,7 +2847,7 @@
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B218" s="2">
         <v>45436</v>
@@ -2852,7 +2858,7 @@
     </row>
     <row r="219" spans="1:5">
       <c r="A219" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B219" s="2">
         <v>45446</v>
@@ -2863,7 +2869,7 @@
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B220" s="2">
         <v>45457</v>
@@ -2874,7 +2880,7 @@
     </row>
     <row r="221" spans="1:5">
       <c r="A221" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B221" s="2">
         <v>45468</v>
@@ -2885,7 +2891,7 @@
     </row>
     <row r="222" spans="1:5">
       <c r="A222" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B222" s="2">
         <v>45483</v>
@@ -2896,7 +2902,7 @@
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B223" s="2">
         <v>45496</v>
@@ -2907,7 +2913,7 @@
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B224" s="2">
         <v>45512</v>
@@ -2918,7 +2924,7 @@
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B225" s="2">
         <v>45522</v>
@@ -2929,7 +2935,7 @@
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B226" s="2">
         <v>45532</v>
@@ -2940,7 +2946,7 @@
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B227" s="2">
         <v>45549</v>
@@ -2951,7 +2957,7 @@
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B228" s="2">
         <v>45467</v>
@@ -2962,7 +2968,7 @@
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B229" s="2">
         <v>45477</v>
@@ -2973,7 +2979,7 @@
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B230" s="2">
         <v>45488</v>
@@ -2984,7 +2990,7 @@
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B231" s="2">
         <v>45499</v>
@@ -2995,7 +3001,7 @@
     </row>
     <row r="232" spans="1:5">
       <c r="A232" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B232" s="2">
         <v>45513</v>
@@ -3006,7 +3012,7 @@
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B233" s="2">
         <v>45523</v>
@@ -3017,7 +3023,7 @@
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B234" s="2">
         <v>45535</v>
@@ -3028,7 +3034,7 @@
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B235" s="2">
         <v>45549</v>
@@ -3039,7 +3045,7 @@
     </row>
     <row r="236" spans="1:5">
       <c r="A236" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B236" s="2">
         <v>45436</v>
@@ -3050,7 +3056,7 @@
     </row>
     <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B237" s="2">
         <v>45446</v>
@@ -3061,7 +3067,7 @@
     </row>
     <row r="238" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B238" s="2">
         <v>45457</v>
@@ -3072,7 +3078,7 @@
     </row>
     <row r="239" spans="1:5">
       <c r="A239" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B239" s="2">
         <v>45468</v>
@@ -3083,7 +3089,7 @@
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B240" s="2">
         <v>45483</v>
@@ -3094,7 +3100,7 @@
     </row>
     <row r="241" spans="1:5">
       <c r="A241" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B241" s="2">
         <v>45496</v>
@@ -3105,7 +3111,7 @@
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B242" s="2">
         <v>45512</v>
@@ -3116,7 +3122,7 @@
     </row>
     <row r="243" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B243" s="2">
         <v>45522</v>
@@ -3127,7 +3133,7 @@
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B244" s="2">
         <v>45532</v>
@@ -3138,7 +3144,7 @@
     </row>
     <row r="245" spans="1:5">
       <c r="A245" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B245" s="2">
         <v>45549</v>
@@ -3149,7 +3155,7 @@
     </row>
     <row r="246" spans="1:5">
       <c r="A246" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B246" s="2">
         <v>45559</v>
@@ -3160,7 +3166,7 @@
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B247" s="2">
         <v>45467</v>
@@ -3171,7 +3177,7 @@
     </row>
     <row r="248" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B248" s="2">
         <v>45477</v>
@@ -3182,7 +3188,7 @@
     </row>
     <row r="249" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B249" s="2">
         <v>45488</v>
@@ -3193,7 +3199,7 @@
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B250" s="2">
         <v>45499</v>
@@ -3204,7 +3210,7 @@
     </row>
     <row r="251" spans="1:5">
       <c r="A251" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B251" s="2">
         <v>45513</v>
@@ -3215,7 +3221,7 @@
     </row>
     <row r="252" spans="1:5">
       <c r="A252" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B252" s="2">
         <v>45523</v>
@@ -3226,7 +3232,7 @@
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B253" s="2">
         <v>45535</v>
@@ -3237,7 +3243,7 @@
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B254" s="2">
         <v>45549</v>
@@ -3248,7 +3254,7 @@
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B255" s="2">
         <v>45467</v>
@@ -3259,7 +3265,7 @@
     </row>
     <row r="256" spans="1:5">
       <c r="A256" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B256" s="2">
         <v>45477</v>
@@ -3270,7 +3276,7 @@
     </row>
     <row r="257" spans="1:5">
       <c r="A257" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B257" s="2">
         <v>45488</v>
@@ -3281,7 +3287,7 @@
     </row>
     <row r="258" spans="1:5">
       <c r="A258" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B258" s="2">
         <v>45499</v>
@@ -3292,7 +3298,7 @@
     </row>
     <row r="259" spans="1:5">
       <c r="A259" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B259" s="2">
         <v>45513</v>
@@ -3303,7 +3309,7 @@
     </row>
     <row r="260" spans="1:5">
       <c r="A260" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B260" s="2">
         <v>45523</v>
@@ -3314,7 +3320,7 @@
     </row>
     <row r="261" spans="1:5">
       <c r="A261" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B261" s="2">
         <v>45535</v>
@@ -3325,7 +3331,7 @@
     </row>
     <row r="262" spans="1:5">
       <c r="A262" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B262" s="2">
         <v>45549</v>
@@ -3336,7 +3342,7 @@
     </row>
     <row r="263" spans="1:5">
       <c r="A263" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B263" s="2">
         <v>45436</v>
@@ -3347,7 +3353,7 @@
     </row>
     <row r="264" spans="1:5">
       <c r="A264" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B264" s="2">
         <v>45446</v>
@@ -3358,7 +3364,7 @@
     </row>
     <row r="265" spans="1:5">
       <c r="A265" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B265" s="2">
         <v>45457</v>
@@ -3369,7 +3375,7 @@
     </row>
     <row r="266" spans="1:5">
       <c r="A266" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B266" s="2">
         <v>45468</v>
@@ -3380,7 +3386,7 @@
     </row>
     <row r="267" spans="1:5">
       <c r="A267" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B267" s="2">
         <v>45483</v>
@@ -3391,7 +3397,7 @@
     </row>
     <row r="268" spans="1:5">
       <c r="A268" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B268" s="2">
         <v>45496</v>
@@ -3402,7 +3408,7 @@
     </row>
     <row r="269" spans="1:5">
       <c r="A269" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B269" s="2">
         <v>45512</v>
@@ -3413,7 +3419,7 @@
     </row>
     <row r="270" spans="1:5">
       <c r="A270" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B270" s="2">
         <v>45522</v>
@@ -3424,7 +3430,7 @@
     </row>
     <row r="271" spans="1:5">
       <c r="A271" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B271" s="2">
         <v>45532</v>
@@ -3435,7 +3441,7 @@
     </row>
     <row r="272" spans="1:5">
       <c r="A272" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B272" s="2">
         <v>45549</v>
@@ -3446,7 +3452,7 @@
     </row>
     <row r="273" spans="1:5">
       <c r="A273" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B273" s="2">
         <v>45436</v>
@@ -3457,7 +3463,7 @@
     </row>
     <row r="274" spans="1:5">
       <c r="A274" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B274" s="2">
         <v>45446</v>
@@ -3468,7 +3474,7 @@
     </row>
     <row r="275" spans="1:5">
       <c r="A275" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B275" s="2">
         <v>45457</v>
@@ -3479,7 +3485,7 @@
     </row>
     <row r="276" spans="1:5">
       <c r="A276" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B276" s="2">
         <v>45468</v>
@@ -3490,7 +3496,7 @@
     </row>
     <row r="277" spans="1:5">
       <c r="A277" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B277" s="2">
         <v>45483</v>
@@ -3501,7 +3507,7 @@
     </row>
     <row r="278" spans="1:5">
       <c r="A278" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B278" s="2">
         <v>45496</v>
@@ -3512,7 +3518,7 @@
     </row>
     <row r="279" spans="1:5">
       <c r="A279" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B279" s="2">
         <v>45512</v>
@@ -3523,7 +3529,7 @@
     </row>
     <row r="280" spans="1:5">
       <c r="A280" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B280" s="2">
         <v>45522</v>
@@ -3534,7 +3540,7 @@
     </row>
     <row r="281" spans="1:5">
       <c r="A281" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B281" s="2">
         <v>45532</v>
@@ -3545,7 +3551,7 @@
     </row>
     <row r="282" spans="1:5">
       <c r="A282" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B282" s="2">
         <v>45549</v>
@@ -3556,7 +3562,7 @@
     </row>
     <row r="283" spans="1:5">
       <c r="A283" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B283" s="2">
         <v>45436</v>
@@ -3567,7 +3573,7 @@
     </row>
     <row r="284" spans="1:5">
       <c r="A284" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B284" s="2">
         <v>45446</v>
@@ -3578,7 +3584,7 @@
     </row>
     <row r="285" spans="1:5">
       <c r="A285" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B285" s="2">
         <v>45457</v>
@@ -3589,7 +3595,7 @@
     </row>
     <row r="286" spans="1:5">
       <c r="A286" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B286" s="2">
         <v>45468</v>
@@ -3600,7 +3606,7 @@
     </row>
     <row r="287" spans="1:5">
       <c r="A287" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B287" s="2">
         <v>45483</v>
@@ -3611,7 +3617,7 @@
     </row>
     <row r="288" spans="1:5">
       <c r="A288" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B288" s="2">
         <v>45496</v>
@@ -3622,7 +3628,7 @@
     </row>
     <row r="289" spans="1:5">
       <c r="A289" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B289" s="2">
         <v>45512</v>
@@ -3633,7 +3639,7 @@
     </row>
     <row r="290" spans="1:5">
       <c r="A290" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B290" s="2">
         <v>45522</v>
@@ -3644,7 +3650,7 @@
     </row>
     <row r="291" spans="1:5">
       <c r="A291" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B291" s="2">
         <v>45532</v>
@@ -3655,7 +3661,7 @@
     </row>
     <row r="292" spans="1:5">
       <c r="A292" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B292" s="2">
         <v>45549</v>
@@ -3666,7 +3672,7 @@
     </row>
     <row r="293" spans="1:5">
       <c r="A293" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B293" s="2">
         <v>45467</v>
@@ -3677,7 +3683,7 @@
     </row>
     <row r="294" spans="1:5">
       <c r="A294" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B294" s="2">
         <v>45477</v>
@@ -3688,7 +3694,7 @@
     </row>
     <row r="295" spans="1:5">
       <c r="A295" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B295" s="2">
         <v>45488</v>
@@ -3699,7 +3705,7 @@
     </row>
     <row r="296" spans="1:5">
       <c r="A296" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B296" s="2">
         <v>45499</v>
@@ -3710,7 +3716,7 @@
     </row>
     <row r="297" spans="1:5">
       <c r="A297" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B297" s="2">
         <v>45513</v>
@@ -3721,7 +3727,7 @@
     </row>
     <row r="298" spans="1:5">
       <c r="A298" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B298" s="2">
         <v>45523</v>
@@ -3732,7 +3738,7 @@
     </row>
     <row r="299" spans="1:5">
       <c r="A299" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B299" s="2">
         <v>45535</v>
@@ -3743,7 +3749,7 @@
     </row>
     <row r="300" spans="1:5">
       <c r="A300" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B300" s="2">
         <v>45549</v>
@@ -3754,7 +3760,7 @@
     </row>
     <row r="301" spans="1:5">
       <c r="A301" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B301" s="2">
         <v>45467</v>
@@ -3765,7 +3771,7 @@
     </row>
     <row r="302" spans="1:5">
       <c r="A302" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B302" s="2">
         <v>45477</v>
@@ -3776,7 +3782,7 @@
     </row>
     <row r="303" spans="1:5">
       <c r="A303" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B303" s="2">
         <v>45488</v>
@@ -3787,7 +3793,7 @@
     </row>
     <row r="304" spans="1:5">
       <c r="A304" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B304" s="2">
         <v>45499</v>
@@ -3798,7 +3804,7 @@
     </row>
     <row r="305" spans="1:5">
       <c r="A305" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B305" s="2">
         <v>45513</v>
@@ -3809,7 +3815,7 @@
     </row>
     <row r="306" spans="1:5">
       <c r="A306" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B306" s="2">
         <v>45523</v>
@@ -3820,7 +3826,7 @@
     </row>
     <row r="307" spans="1:5">
       <c r="A307" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B307" s="2">
         <v>45535</v>
@@ -3831,7 +3837,7 @@
     </row>
     <row r="308" spans="1:5">
       <c r="A308" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B308" s="2">
         <v>45549</v>
@@ -3842,7 +3848,7 @@
     </row>
     <row r="309" spans="1:5">
       <c r="A309" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B309" s="2">
         <v>45559</v>
@@ -3853,7 +3859,7 @@
     </row>
     <row r="310" spans="1:5">
       <c r="A310" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B310" s="2">
         <v>45436</v>
@@ -3864,7 +3870,7 @@
     </row>
     <row r="311" spans="1:5">
       <c r="A311" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B311" s="2">
         <v>45446</v>
@@ -3875,7 +3881,7 @@
     </row>
     <row r="312" spans="1:5">
       <c r="A312" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B312" s="2">
         <v>45457</v>
@@ -3886,7 +3892,7 @@
     </row>
     <row r="313" spans="1:5">
       <c r="A313" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B313" s="2">
         <v>45468</v>
@@ -3897,7 +3903,7 @@
     </row>
     <row r="314" spans="1:5">
       <c r="A314" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B314" s="2">
         <v>45483</v>
@@ -3908,7 +3914,7 @@
     </row>
     <row r="315" spans="1:5">
       <c r="A315" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B315" s="2">
         <v>45496</v>
@@ -3919,7 +3925,7 @@
     </row>
     <row r="316" spans="1:5">
       <c r="A316" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B316" s="2">
         <v>45512</v>
@@ -3930,7 +3936,7 @@
     </row>
     <row r="317" spans="1:5">
       <c r="A317" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B317" s="2">
         <v>45522</v>
@@ -3941,7 +3947,7 @@
     </row>
     <row r="318" spans="1:5">
       <c r="A318" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B318" s="2">
         <v>45532</v>
@@ -3952,7 +3958,7 @@
     </row>
     <row r="319" spans="1:5">
       <c r="A319" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B319" s="2">
         <v>45549</v>
@@ -3963,7 +3969,7 @@
     </row>
     <row r="320" spans="1:5">
       <c r="A320" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B320" s="2">
         <v>45436</v>
@@ -3974,7 +3980,7 @@
     </row>
     <row r="321" spans="1:5">
       <c r="A321" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B321" s="2">
         <v>45446</v>
@@ -3985,7 +3991,7 @@
     </row>
     <row r="322" spans="1:5">
       <c r="A322" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B322" s="2">
         <v>45457</v>
@@ -3996,7 +4002,7 @@
     </row>
     <row r="323" spans="1:5">
       <c r="A323" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B323" s="2">
         <v>45468</v>
@@ -4007,7 +4013,7 @@
     </row>
     <row r="324" spans="1:5">
       <c r="A324" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B324" s="2">
         <v>45483</v>
@@ -4018,7 +4024,7 @@
     </row>
     <row r="325" spans="1:5">
       <c r="A325" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B325" s="2">
         <v>45496</v>
@@ -4029,7 +4035,7 @@
     </row>
     <row r="326" spans="1:5">
       <c r="A326" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B326" s="2">
         <v>45512</v>
@@ -4040,7 +4046,7 @@
     </row>
     <row r="327" spans="1:5">
       <c r="A327" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B327" s="2">
         <v>45522</v>
@@ -4051,7 +4057,7 @@
     </row>
     <row r="328" spans="1:5">
       <c r="A328" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B328" s="2">
         <v>45532</v>
@@ -4062,7 +4068,7 @@
     </row>
     <row r="329" spans="1:5">
       <c r="A329" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B329" s="2">
         <v>45549</v>
@@ -4073,7 +4079,7 @@
     </row>
     <row r="330" spans="1:5">
       <c r="A330" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B330" s="2">
         <v>45467</v>
@@ -4084,7 +4090,7 @@
     </row>
     <row r="331" spans="1:5">
       <c r="A331" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B331" s="2">
         <v>45477</v>
@@ -4095,7 +4101,7 @@
     </row>
     <row r="332" spans="1:5">
       <c r="A332" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B332" s="2">
         <v>45488</v>
@@ -4106,7 +4112,7 @@
     </row>
     <row r="333" spans="1:5">
       <c r="A333" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B333" s="2">
         <v>45499</v>
@@ -4117,7 +4123,7 @@
     </row>
     <row r="334" spans="1:5">
       <c r="A334" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B334" s="2">
         <v>45513</v>
@@ -4128,7 +4134,7 @@
     </row>
     <row r="335" spans="1:5">
       <c r="A335" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B335" s="2">
         <v>45523</v>
@@ -4139,7 +4145,7 @@
     </row>
     <row r="336" spans="1:5">
       <c r="A336" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B336" s="2">
         <v>45535</v>
@@ -4150,7 +4156,7 @@
     </row>
     <row r="337" spans="1:5">
       <c r="A337" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B337" s="2">
         <v>45549</v>
@@ -4161,7 +4167,7 @@
     </row>
     <row r="338" spans="1:5">
       <c r="A338" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B338" s="2">
         <v>45559</v>
@@ -4172,7 +4178,7 @@
     </row>
     <row r="339" spans="1:5">
       <c r="A339" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B339" s="2">
         <v>45436</v>
@@ -4183,7 +4189,7 @@
     </row>
     <row r="340" spans="1:5">
       <c r="A340" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B340" s="2">
         <v>45446</v>
@@ -4194,7 +4200,7 @@
     </row>
     <row r="341" spans="1:5">
       <c r="A341" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B341" s="2">
         <v>45457</v>
@@ -4205,7 +4211,7 @@
     </row>
     <row r="342" spans="1:5">
       <c r="A342" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B342" s="2">
         <v>45468</v>
@@ -4216,7 +4222,7 @@
     </row>
     <row r="343" spans="1:5">
       <c r="A343" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B343" s="2">
         <v>45483</v>
@@ -4227,7 +4233,7 @@
     </row>
     <row r="344" spans="1:5">
       <c r="A344" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B344" s="2">
         <v>45496</v>
@@ -4238,7 +4244,7 @@
     </row>
     <row r="345" spans="1:5">
       <c r="A345" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B345" s="2">
         <v>45512</v>
@@ -4249,7 +4255,7 @@
     </row>
     <row r="346" spans="1:5">
       <c r="A346" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B346" s="2">
         <v>45522</v>
@@ -4260,7 +4266,7 @@
     </row>
     <row r="347" spans="1:5">
       <c r="A347" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B347" s="2">
         <v>45532</v>
@@ -4271,7 +4277,7 @@
     </row>
     <row r="348" spans="1:5">
       <c r="A348" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B348" s="2">
         <v>45549</v>
@@ -4282,7 +4288,7 @@
     </row>
     <row r="349" spans="1:5">
       <c r="A349" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B349" s="2">
         <v>45559</v>
@@ -4293,7 +4299,7 @@
     </row>
     <row r="350" spans="1:5">
       <c r="A350" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B350" s="2">
         <v>45467</v>
@@ -4304,7 +4310,7 @@
     </row>
     <row r="351" spans="1:5">
       <c r="A351" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B351" s="2">
         <v>45477</v>
@@ -4315,7 +4321,7 @@
     </row>
     <row r="352" spans="1:5">
       <c r="A352" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B352" s="2">
         <v>45488</v>
@@ -4324,9 +4330,9 @@
         <v>5.025</v>
       </c>
     </row>
-    <row r="353" spans="1:5">
+    <row r="353" spans="1:6">
       <c r="A353" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B353" s="2">
         <v>45499</v>
@@ -4335,9 +4341,9 @@
         <v>5.941666666666666</v>
       </c>
     </row>
-    <row r="354" spans="1:5">
+    <row r="354" spans="1:6">
       <c r="A354" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B354" s="2">
         <v>45513</v>
@@ -4346,9 +4352,9 @@
         <v>6.891666666666667</v>
       </c>
     </row>
-    <row r="355" spans="1:5">
+    <row r="355" spans="1:6">
       <c r="A355" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B355" s="2">
         <v>45523</v>
@@ -4357,9 +4363,9 @@
         <v>7.875</v>
       </c>
     </row>
-    <row r="356" spans="1:5">
+    <row r="356" spans="1:6">
       <c r="A356" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B356" s="2">
         <v>45535</v>
@@ -4368,15 +4374,543 @@
         <v>9.074999999999999</v>
       </c>
     </row>
-    <row r="357" spans="1:5">
+    <row r="357" spans="1:6">
       <c r="A357" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B357" s="2">
         <v>45549</v>
       </c>
       <c r="E357">
         <v>9.916666666666666</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6">
+      <c r="A358" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B358" s="2">
+        <v>45438</v>
+      </c>
+      <c r="F358">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6">
+      <c r="A359" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B359" s="2">
+        <v>45409</v>
+      </c>
+      <c r="F359">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6">
+      <c r="A360" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B360" s="2">
+        <v>45439</v>
+      </c>
+      <c r="F360">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6">
+      <c r="A361" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B361" s="2">
+        <v>45409</v>
+      </c>
+      <c r="F361">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6">
+      <c r="A362" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B362" s="2">
+        <v>45439</v>
+      </c>
+      <c r="F362">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6">
+      <c r="A363" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B363" s="2">
+        <v>45437</v>
+      </c>
+      <c r="F363">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6">
+      <c r="A364" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B364" s="2">
+        <v>45410</v>
+      </c>
+      <c r="F364">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6">
+      <c r="A365" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B365" s="2">
+        <v>45416</v>
+      </c>
+      <c r="F365">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6">
+      <c r="A366" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B366" s="2">
+        <v>45414</v>
+      </c>
+      <c r="F366">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6">
+      <c r="A367" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B367" s="2">
+        <v>45439</v>
+      </c>
+      <c r="F367">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6">
+      <c r="A368" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B368" s="2">
+        <v>45439</v>
+      </c>
+      <c r="F368">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6">
+      <c r="A369" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B369" s="2">
+        <v>45410</v>
+      </c>
+      <c r="F369">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6">
+      <c r="A370" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B370" s="2">
+        <v>45413</v>
+      </c>
+      <c r="F370">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6">
+      <c r="A371" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B371" s="2">
+        <v>45438</v>
+      </c>
+      <c r="F371">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6">
+      <c r="A372" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B372" s="2">
+        <v>45414</v>
+      </c>
+      <c r="F372">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6">
+      <c r="A373" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B373" s="2">
+        <v>45438</v>
+      </c>
+      <c r="F373">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6">
+      <c r="A374" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B374" s="2">
+        <v>45547</v>
+      </c>
+      <c r="F374">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6">
+      <c r="A375" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B375" s="2">
+        <v>45543</v>
+      </c>
+      <c r="F375">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6">
+      <c r="A376" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B376" s="2">
+        <v>45545</v>
+      </c>
+      <c r="F376">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6">
+      <c r="A377" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B377" s="2">
+        <v>45547</v>
+      </c>
+      <c r="F377">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6">
+      <c r="A378" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B378" s="2">
+        <v>45541</v>
+      </c>
+      <c r="F378">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6">
+      <c r="A379" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B379" s="2">
+        <v>45549</v>
+      </c>
+      <c r="F379">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6">
+      <c r="A380" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B380" s="2">
+        <v>45538</v>
+      </c>
+      <c r="F380">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6">
+      <c r="A381" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B381" s="2">
+        <v>45545</v>
+      </c>
+      <c r="F381">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6">
+      <c r="A382" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B382" s="2">
+        <v>45548</v>
+      </c>
+      <c r="F382">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6">
+      <c r="A383" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B383" s="2">
+        <v>45542</v>
+      </c>
+      <c r="F383">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6">
+      <c r="A384" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B384" s="2">
+        <v>45546</v>
+      </c>
+      <c r="F384">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6">
+      <c r="A385" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B385" s="2">
+        <v>45544</v>
+      </c>
+      <c r="F385">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6">
+      <c r="A386" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B386" s="2">
+        <v>45539</v>
+      </c>
+      <c r="F386">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6">
+      <c r="A387" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B387" s="2">
+        <v>45546</v>
+      </c>
+      <c r="F387">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6">
+      <c r="A388" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B388" s="2">
+        <v>45546</v>
+      </c>
+      <c r="F388">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6">
+      <c r="A389" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B389" s="2">
+        <v>45546</v>
+      </c>
+      <c r="F389">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6">
+      <c r="A390" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B390" s="2">
+        <v>45568</v>
+      </c>
+      <c r="F390">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6">
+      <c r="A391" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B391" s="2">
+        <v>45565</v>
+      </c>
+      <c r="F391">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6">
+      <c r="A392" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B392" s="2">
+        <v>45566</v>
+      </c>
+      <c r="F392">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6">
+      <c r="A393" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B393" s="2">
+        <v>45568</v>
+      </c>
+      <c r="F393">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6">
+      <c r="A394" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B394" s="2">
+        <v>45560</v>
+      </c>
+      <c r="F394">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6">
+      <c r="A395" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B395" s="2">
+        <v>45567</v>
+      </c>
+      <c r="F395">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6">
+      <c r="A396" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B396" s="2">
+        <v>45560</v>
+      </c>
+      <c r="F396">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6">
+      <c r="A397" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B397" s="2">
+        <v>45566</v>
+      </c>
+      <c r="F397">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6">
+      <c r="A398" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B398" s="2">
+        <v>45567</v>
+      </c>
+      <c r="F398">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6">
+      <c r="A399" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B399" s="2">
+        <v>45561</v>
+      </c>
+      <c r="F399">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6">
+      <c r="A400" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B400" s="2">
+        <v>45567</v>
+      </c>
+      <c r="F400">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6">
+      <c r="A401" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B401" s="2">
+        <v>45566</v>
+      </c>
+      <c r="F401">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6">
+      <c r="A402" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B402" s="2">
+        <v>45560</v>
+      </c>
+      <c r="F402">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6">
+      <c r="A403" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B403" s="2">
+        <v>45566</v>
+      </c>
+      <c r="F403">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6">
+      <c r="A404" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B404" s="2">
+        <v>45567</v>
+      </c>
+      <c r="F404">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6">
+      <c r="A405" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B405" s="2">
+        <v>45567</v>
+      </c>
+      <c r="F405">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>